<commit_message>
Changes to the budget of uncertainty
</commit_message>
<xml_diff>
--- a/code/graphs.xlsx
+++ b/code/graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaled\Documents\GitHub\ThermalExpansionUncertainty\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CC7D6B-C96F-436D-9260-D42000556666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE1DAD-411E-48C3-9410-C3D6ECE15359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="134">
   <si>
     <t>SensibilityCoeficientsVariables</t>
   </si>
@@ -1155,13 +1155,46 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>Number of Transitions N</t>
+  </si>
+  <si>
+    <t>Maximum N Error</t>
+  </si>
+  <si>
+    <t>Wavelength λ</t>
+  </si>
+  <si>
+    <t>Maximum λ Error</t>
+  </si>
+  <si>
+    <t>Initial Length L0</t>
+  </si>
+  <si>
+    <t>Maximum L0 Error</t>
+  </si>
+  <si>
+    <t>Object Temperature T</t>
+  </si>
+  <si>
+    <t>60 °C</t>
+  </si>
+  <si>
+    <t>Maximum T Error</t>
+  </si>
+  <si>
+    <t>Temperature of Reference T0</t>
+  </si>
+  <si>
+    <t>Maximum T0 Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="General&quot; °C^-1&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;± &quot;General"/>
     <numFmt numFmtId="166" formatCode="General&quot; m&quot;"/>
@@ -1172,8 +1205,9 @@
     <numFmt numFmtId="171" formatCode="General&quot; °C^-2&quot;"/>
     <numFmt numFmtId="172" formatCode="&quot;± &quot;General&quot; °C&quot;"/>
     <numFmt numFmtId="173" formatCode="0.000E+00&quot; °C^-1&quot;"/>
+    <numFmt numFmtId="176" formatCode="&quot;± &quot;General\ &quot;%&quot;"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1249,6 +1283,24 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="DejaVu Sans"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1387,7 +1439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1504,15 +1556,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1522,9 +1580,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1558,7 +1613,65 @@
     <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1734,6 +1847,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-6428-46AF-A650-2F3FC9CFF381}"/>
                 </c:ext>
@@ -2220,6 +2334,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-C6A2-42F3-A50A-A68BADA85E3E}"/>
                 </c:ext>
@@ -3387,7 +3502,7 @@
         <v>8.9970906575520802E-14</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F2:F31" si="0">SQRT(E3)</f>
+        <f t="shared" ref="F3:F31" si="0">SQRT(E3)</f>
         <v>2.9995150703992272E-7</v>
       </c>
       <c r="G3" s="3"/>
@@ -4854,23 +4969,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:I31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="74" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="42.75" customHeight="1">
@@ -5375,320 +5490,300 @@
       <c r="A19" s="13">
         <v>1</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="44">
+      <c r="C19" s="47">
         <v>125</v>
       </c>
-      <c r="D19" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="44">
+      <c r="D19" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="47">
         <f>1/SQRT(3)</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="H19" s="45">
-        <f>Data!D19</f>
-        <v>2.10869312286377E-5</v>
-      </c>
-      <c r="I19" s="46">
-        <f>Data!F19</f>
-        <v>3.8267090615971189E-12</v>
+      <c r="H19" s="48">
+        <v>8.3124999999999998E-8</v>
+      </c>
+      <c r="I19" s="44">
+        <v>4.799224112638761E-8</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="47" t="s">
+      <c r="C20" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="50">
         <v>1</v>
       </c>
-      <c r="F20" s="47" t="s">
+      <c r="F20" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="49">
         <f>1/SQRT(3)</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="H20" s="49">
-        <f>Data!D19</f>
-        <v>2.10869312286377E-5</v>
-      </c>
-      <c r="I20" s="50">
-        <f>Data!F19</f>
-        <v>3.8267090615971189E-12</v>
+      <c r="H20" s="51">
+        <v>8.3124999999999998E-8</v>
+      </c>
+      <c r="I20" s="45">
+        <v>4.799224112638761E-8</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="13">
         <v>2</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="51">
+      <c r="D21" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="52">
         <f>5*10^(-9) /SQRT(3)</f>
         <v>2.8867513459481292E-9</v>
       </c>
-      <c r="H21" s="52">
-        <f>Data!D20</f>
-        <v>2.6358664035797101E-11</v>
-      </c>
-      <c r="I21" s="46">
-        <f>Data!F20</f>
-        <v>4.2783907959227964E-11</v>
+      <c r="H21" s="53">
+        <v>19.53125</v>
+      </c>
+      <c r="I21" s="44">
+        <v>2.9995150703992272E-7</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="47" t="s">
+      <c r="C22" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="53">
+      <c r="E22" s="54">
         <v>5</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="54">
+      <c r="G22" s="55">
         <f>5*10^(-9) /SQRT(3)</f>
         <v>2.8867513459481292E-9</v>
       </c>
-      <c r="H22" s="55">
-        <f>Data!D20</f>
-        <v>2.6358664035797101E-11</v>
-      </c>
-      <c r="I22" s="50">
-        <f>Data!F20</f>
-        <v>4.2783907959227964E-11</v>
+      <c r="H22" s="56">
+        <v>19.53125</v>
+      </c>
+      <c r="I22" s="45">
+        <v>2.9995150703992272E-7</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.6">
       <c r="A23" s="13">
         <v>3</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="51">
+      <c r="D23" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="52">
         <f>0.05*10^(-3) /SQRT(3)</f>
         <v>2.8867513459481293E-5</v>
       </c>
-      <c r="H23" s="52">
-        <f>Data!D21</f>
-        <v>2.6358664035797101E-11</v>
-      </c>
-      <c r="I23" s="46">
-        <f>Data!F21</f>
-        <v>4.2783907959227964E-11</v>
+      <c r="H23" s="53">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="I23" s="44">
+        <v>3.7493938379990304E-9</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.6">
       <c r="A24" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="47" t="s">
+      <c r="C24" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="57">
         <v>0.05</v>
       </c>
-      <c r="F24" s="47" t="s">
+      <c r="F24" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="55">
         <f>0.05*10^(-3) /SQRT(3)</f>
         <v>2.8867513459481293E-5</v>
       </c>
-      <c r="H24" s="55">
-        <f>Data!D21</f>
-        <v>2.6358664035797101E-11</v>
-      </c>
-      <c r="I24" s="50">
-        <f>Data!F21</f>
-        <v>4.2783907959227964E-11</v>
+      <c r="H24" s="56">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="I24" s="45">
+        <v>3.7493938379990304E-9</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="13.8">
       <c r="A25" s="13">
         <v>4</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="44" t="s">
+      <c r="C25" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="57">
+      <c r="D25" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="58">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H25" s="58">
-        <f>Data!D22</f>
-        <v>2.1593017578124998E-18</v>
-      </c>
-      <c r="I25" s="46">
-        <f>Data!F22</f>
-        <v>2.4490937994221576E-10</v>
+      <c r="H25" s="59">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="I25" s="44">
+        <v>7.4987876759980681E-8</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="47" t="s">
+      <c r="C26" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="59">
+      <c r="E26" s="60">
         <v>0.5</v>
       </c>
-      <c r="F26" s="47" t="s">
+      <c r="F26" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="G26" s="60">
+      <c r="G26" s="61">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H26" s="61">
-        <f>Data!D22</f>
-        <v>2.1593017578124998E-18</v>
-      </c>
-      <c r="I26" s="50">
-        <f>Data!F22</f>
-        <v>2.4490937994221576E-10</v>
+      <c r="H26" s="62">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="I26" s="45">
+        <v>7.4987876759980681E-8</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.6">
       <c r="A27" s="13">
         <v>5</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="57">
+      <c r="D27" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="58">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H27" s="58">
-        <f>Data!D23</f>
-        <v>0.119209289550781</v>
-      </c>
-      <c r="I27" s="46">
-        <f>Data!F23</f>
-        <v>1.5306836246388474E-9</v>
+      <c r="H27" s="59">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="I27" s="44">
+        <v>7.4987876759980681E-8</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.6">
       <c r="A28" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="47" t="s">
+      <c r="C28" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="59">
+      <c r="E28" s="60">
         <v>0.5</v>
       </c>
-      <c r="F28" s="47" t="s">
+      <c r="F28" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="G28" s="60">
+      <c r="G28" s="61">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H28" s="61">
-        <f>Data!D23</f>
-        <v>0.119209289550781</v>
-      </c>
-      <c r="I28" s="50">
-        <f>Data!F23</f>
-        <v>1.5306836246388474E-9</v>
+      <c r="H28" s="62">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="I28" s="45">
+        <v>7.4987876759980681E-8</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -5717,7 +5812,7 @@
       <c r="H29" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="I29" s="62">
+      <c r="I29" s="46">
         <v>3.2183031781572201E-7</v>
       </c>
     </row>
@@ -5738,9 +5833,374 @@
         <v>6.4366063563144401E-7</v>
       </c>
     </row>
+    <row r="34" spans="1:9" ht="98.4">
+      <c r="A34" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="I34" s="65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="24.6">
+      <c r="A35" s="66">
+        <v>1</v>
+      </c>
+      <c r="B35" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="66">
+        <v>125</v>
+      </c>
+      <c r="D35" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="67">
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="H35" s="68">
+        <v>8.3124999999999998E-8</v>
+      </c>
+      <c r="I35" s="68">
+        <v>4.799224112638761E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="24.6">
+      <c r="A36" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="70">
+        <v>1</v>
+      </c>
+      <c r="F36" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G36" s="71">
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="H36" s="72">
+        <v>8.3124999999999998E-8</v>
+      </c>
+      <c r="I36" s="73">
+        <v>4.799224112638761E-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="24.6">
+      <c r="A37" s="66">
+        <v>2</v>
+      </c>
+      <c r="B37" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="67">
+        <v>2.8867513459481292E-9</v>
+      </c>
+      <c r="H37" s="74">
+        <v>19.53125</v>
+      </c>
+      <c r="I37" s="68">
+        <v>2.9995150703992272E-7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="24.6">
+      <c r="A38" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G38" s="71">
+        <v>2.8867513459481292E-9</v>
+      </c>
+      <c r="H38" s="76">
+        <v>19.53125</v>
+      </c>
+      <c r="I38" s="73">
+        <v>2.9995150703992272E-7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="24.6">
+      <c r="A39" s="66">
+        <v>3</v>
+      </c>
+      <c r="B39" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="67">
+        <v>2.8867513459481293E-5</v>
+      </c>
+      <c r="H39" s="74">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="I39" s="68">
+        <v>3.7493938379990304E-9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="24.6">
+      <c r="A40" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="77">
+        <v>0.05</v>
+      </c>
+      <c r="F40" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="71">
+        <v>2.8867513459481293E-5</v>
+      </c>
+      <c r="H40" s="76">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="I40" s="73">
+        <v>3.7493938379990304E-9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="24.6">
+      <c r="A41" s="66">
+        <v>4</v>
+      </c>
+      <c r="B41" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="67">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H41" s="78">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="I41" s="68">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="24.6">
+      <c r="A42" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="F42" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G42" s="71">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H42" s="80">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="I42" s="73">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="24.6">
+      <c r="A43" s="66">
+        <v>5</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="67">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H43" s="78">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="I43" s="68">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="24.6">
+      <c r="A44" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="71">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="H44" s="80">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="I44" s="73">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="24.6">
+      <c r="A45" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="81">
+        <v>1.039E-5</v>
+      </c>
+      <c r="D45" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="H45" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="83">
+        <v>3.2183031781572201E-7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="H46" s="63" t="s">
+        <v>119</v>
+      </c>
+      <c r="I46" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="H47" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" s="43">
+        <f>I45*2</f>
+        <v>6.4366063563144401E-7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
New lambda uncertainty and final budget format
</commit_message>
<xml_diff>
--- a/code/graphs.xlsx
+++ b/code/graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaled\Documents\GitHub\ThermalExpansionUncertainty\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22094155-8041-4819-89C2-C93B6134773A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DF716-BB00-4AC2-A0E9-3FA5CED8E873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="135">
   <si>
     <t>SensibilityCoeficientsVariables</t>
   </si>
@@ -1188,6 +1188,9 @@
   </si>
   <si>
     <t>Maximum T0 Error</t>
+  </si>
+  <si>
+    <t>0.00001039 ℃^(−1)</t>
   </si>
 </sst>
 </file>
@@ -1199,16 +1202,16 @@
     <numFmt numFmtId="165" formatCode="&quot;± &quot;General"/>
     <numFmt numFmtId="166" formatCode="General&quot; m&quot;"/>
     <numFmt numFmtId="167" formatCode="General&quot; m^-1 °C^-1&quot;"/>
-    <numFmt numFmtId="168" formatCode="&quot;± &quot;General&quot; nm&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;± &quot;General&quot; mm&quot;"/>
     <numFmt numFmtId="170" formatCode="General&quot; °C&quot;"/>
     <numFmt numFmtId="171" formatCode="General&quot; °C^-2&quot;"/>
     <numFmt numFmtId="172" formatCode="&quot;± &quot;General&quot; °C&quot;"/>
     <numFmt numFmtId="173" formatCode="0.000E+00&quot; °C^-1&quot;"/>
     <numFmt numFmtId="174" formatCode="&quot;± &quot;General\ &quot;%&quot;"/>
-    <numFmt numFmtId="175" formatCode="0.00E+00\ &quot; m^-1 °C^-1&quot;"/>
+    <numFmt numFmtId="178" formatCode="&quot;k= &quot;General"/>
+    <numFmt numFmtId="179" formatCode="&quot;U= &quot;General&quot; °C^-1&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1284,24 +1287,6 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="DejaVu Sans"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1440,7 +1425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1499,9 +1484,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1566,71 +1548,64 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="179" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="175" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2829,7 +2804,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="2600" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="2600" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Temperature  / °C</a:t>
@@ -2896,7 +2871,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="2600" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="2600" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Length / mm</a:t>
@@ -3051,6 +3026,178 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>64168</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>132347</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="409984" cy="347211"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF7C19B6-548D-C811-217B-979D780EC72E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7002379" y="3332747"/>
+              <a:ext cx="409984" cy="347211"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>℃</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="0">
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF7C19B6-548D-C811-217B-979D780EC72E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7002379" y="3332747"/>
+              <a:ext cx="409984" cy="347211"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>℃</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^(−1)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="0">
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3390,8 +3537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="131" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView zoomScale="131" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -3458,11 +3605,11 @@
         <v>19.53125</v>
       </c>
       <c r="E3" s="2">
-        <v>8.9970906575520802E-14</v>
+        <v>7.94728597005208E-14</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F31" si="0">SQRT(E3)</f>
-        <v>2.9995150703992272E-7</v>
+        <f>SQRT(E3)</f>
+        <v>2.8190931112774692E-7</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -3483,7 +3630,7 @@
         <v>1.4057954152425101E-17</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F3:F31" si="0">SQRT(E4)</f>
         <v>3.7493938379990304E-9</v>
       </c>
       <c r="G4" s="3"/>
@@ -3568,11 +3715,11 @@
         <v>1.220703125E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>9.5968967013889009E-19</v>
+        <v>8.4771050347222299E-19</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>9.7963751976886325E-10</v>
+        <v>9.2071195466998414E-10</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -3656,11 +3803,11 @@
         <v>1.220703125E-2</v>
       </c>
       <c r="E12" s="2">
-        <v>9.5968967013889009E-19</v>
+        <v>8.4771050347222299E-19</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>9.7963751976886325E-10</v>
+        <v>9.2071195466998414E-10</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -3700,11 +3847,11 @@
         <v>149011.611938477</v>
       </c>
       <c r="E14" s="2">
-        <v>2.9287404484218998E-20</v>
+        <v>2.58700715170966E-20</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>1.7113563183691173E-10</v>
+        <v>1.6084175924521779E-10</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -3722,11 +3869,11 @@
         <v>0.59604644775390603</v>
       </c>
       <c r="E15" s="2">
-        <v>1.17149617936876E-17</v>
+        <v>1.03480286068387E-17</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.4227126367382348E-9</v>
+        <v>3.2168351849043649E-9</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -3744,11 +3891,11 @@
         <v>0.59604644775390603</v>
       </c>
       <c r="E16" s="2">
-        <v>1.17149617936876E-17</v>
+        <v>1.03480286068387E-17</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>3.4227126367382348E-9</v>
+        <v>3.2168351849043649E-9</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -3788,11 +3935,11 @@
         <v>29802.322387695302</v>
       </c>
       <c r="E18" s="2">
-        <v>5.8574808968438099E-21</v>
+        <v>5.1740143034193303E-21</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>7.6534181231942435E-11</v>
+        <v>7.1930621458592519E-11</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -3898,11 +4045,11 @@
         <v>0.119209289550781</v>
       </c>
       <c r="E23" s="2">
-        <v>2.3429923587375198E-18</v>
+        <v>2.0696057213677299E-18</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>1.5306836246388474E-9</v>
+        <v>1.4386124291718497E-9</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -4008,11 +4155,11 @@
         <v>0.119209289550781</v>
       </c>
       <c r="E28" s="2">
-        <v>2.3429923587375198E-18</v>
+        <v>2.0696057213677299E-18</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>1.5306836246388474E-9</v>
+        <v>1.4386124291718497E-9</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -4928,10 +5075,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="74" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:I45"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -5045,7 +5192,7 @@
         <f>Data!D2</f>
         <v>8.3124999999999998E-8</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="41">
         <f>Data!F2</f>
         <v>4.799224112638761E-8</v>
       </c>
@@ -5082,7 +5229,7 @@
       </c>
       <c r="I4" s="15">
         <f>Data!F3</f>
-        <v>2.9995150703992272E-7</v>
+        <v>2.8190931112774692E-7</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>93</v>
@@ -5101,23 +5248,23 @@
       <c r="D5" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="24">
-        <v>5</v>
+      <c r="E5" s="46">
+        <v>25</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <f>5*10^(-9) /SQRT(3)</f>
         <v>2.8867513459481292E-9</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <f>Data!D3</f>
         <v>19.53125</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="41">
         <f>Data!F3</f>
-        <v>2.9995150703992272E-7</v>
+        <v>2.8190931112774692E-7</v>
       </c>
       <c r="J5" s="21" t="s">
         <v>93</v>
@@ -5171,21 +5318,21 @@
       <c r="D7" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>0.05</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <f>0.05*10^(-3) /SQRT(3)</f>
         <v>2.8867513459481293E-5</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="25">
         <f>Data!D4</f>
         <v>-1.2988281250000001E-4</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="41">
         <f>Data!F4</f>
         <v>3.7493938379990304E-9</v>
       </c>
@@ -5212,11 +5359,11 @@
       <c r="F8" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="28">
         <f>Data!D5</f>
         <v>-2.5976562500000001E-7</v>
       </c>
@@ -5241,21 +5388,21 @@
       <c r="D9" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>0.5</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="30">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <f>Data!D5</f>
         <v>-2.5976562500000001E-7</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="41">
         <f>Data!F5</f>
         <v>7.4987876759980681E-8</v>
       </c>
@@ -5282,11 +5429,11 @@
       <c r="F10" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="28">
         <f>Data!D6</f>
         <v>2.5976562500000001E-7</v>
       </c>
@@ -5311,21 +5458,21 @@
       <c r="D11" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>0.5</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="30">
         <f>0.5 /SQRT(3)</f>
         <v>0.28867513459481292</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="31">
         <f>Data!D6</f>
         <v>2.5976562500000001E-7</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="41">
         <f>Data!F6</f>
         <v>7.4987876759980681E-8</v>
       </c>
@@ -5360,801 +5507,408 @@
       </c>
       <c r="I12" s="20">
         <f>SUM(Data!F7:F31)</f>
-        <v>2.003614818854632E-8</v>
+        <v>1.9307502331381792E-8</v>
       </c>
       <c r="J12" s="21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <f>1.039 *10^-5</f>
         <v>1.039E-5</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="I13" s="37">
-        <v>3.2183031781572201E-7</v>
-      </c>
-      <c r="J13" s="38" t="s">
+      <c r="I13" s="36">
+        <v>3.0507900270517998E-7</v>
+      </c>
+      <c r="J13" s="37" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="40">
+      <c r="I14" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="42">
         <f>I13*2</f>
-        <v>6.4366063563144401E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="9" t="s">
+        <v>6.1015800541035996E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="13">
+    <row r="20" spans="1:8">
+      <c r="A20" s="13">
         <v>1</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="14">
+      <c r="B20" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="49">
         <v>125</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D20" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E20" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F20" s="49">
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="G20" s="50">
+        <v>8.3124999999999998E-8</v>
+      </c>
+      <c r="H20" s="43">
+        <v>4.799224112638761E-8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="14">
-        <f>1/SQRT(3)</f>
+      <c r="D21" s="52">
+        <v>1</v>
+      </c>
+      <c r="E21" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="51">
         <v>0.57735026918962584</v>
       </c>
-      <c r="H19" s="15">
+      <c r="G21" s="53">
         <v>8.3124999999999998E-8</v>
       </c>
-      <c r="I19" s="44">
+      <c r="H21" s="44">
         <v>4.799224112638761E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="18" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="13">
+        <v>2</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="19">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="E22" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="54">
+        <v>2.8867513459481292E-9</v>
+      </c>
+      <c r="G22" s="55">
+        <v>19.53125</v>
+      </c>
+      <c r="H22" s="43">
+        <v>2.8190931112774692E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="56">
+        <v>25</v>
+      </c>
+      <c r="E23" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="18">
-        <f>1/SQRT(3)</f>
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="H20" s="20">
-        <v>8.3124999999999998E-8</v>
-      </c>
-      <c r="I20" s="45">
-        <v>4.799224112638761E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="13">
+      <c r="F23" s="57">
+        <v>2.8867513459481292E-9</v>
+      </c>
+      <c r="G23" s="58">
+        <v>19.53125</v>
+      </c>
+      <c r="H23" s="44">
+        <v>2.8190931112774692E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="13">
+        <v>3</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="54">
+        <v>2.8867513459481293E-5</v>
+      </c>
+      <c r="G24" s="55">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="H24" s="43">
+        <v>3.7493938379990304E-9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="59">
+        <v>0.05</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="57">
+        <v>2.8867513459481293E-5</v>
+      </c>
+      <c r="G25" s="58">
+        <v>-1.2988281250000001E-4</v>
+      </c>
+      <c r="H25" s="44">
+        <v>3.7493938379990304E-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="13">
+        <v>4</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="60">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G26" s="61">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="H26" s="43">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="F27" s="63">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G27" s="64">
+        <v>-2.5976562500000001E-7</v>
+      </c>
+      <c r="H27" s="44">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="13">
+        <v>5</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="60">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G28" s="61">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="H28" s="43">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="62">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="63">
+        <v>0.28867513459481292</v>
+      </c>
+      <c r="G29" s="64">
+        <v>2.5976562500000001E-7</v>
+      </c>
+      <c r="H29" s="44">
+        <v>7.4987876759980681E-8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="17">
+        <v>6</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="H30" s="65">
+        <v>1.9307502331381792E-8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="H31" s="45">
+        <v>3.0507900270517998E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="H32" s="47">
         <v>2</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="22">
-        <f>5*10^(-9) /SQRT(3)</f>
-        <v>2.8867513459481292E-9</v>
-      </c>
-      <c r="H21" s="23">
-        <v>19.53125</v>
-      </c>
-      <c r="I21" s="44">
-        <v>2.9995150703992272E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="24">
-        <v>5</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="25">
-        <f>5*10^(-9) /SQRT(3)</f>
-        <v>2.8867513459481292E-9</v>
-      </c>
-      <c r="H22" s="26">
-        <v>19.53125</v>
-      </c>
-      <c r="I22" s="45">
-        <v>2.9995150703992272E-7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.6">
-      <c r="A23" s="13">
-        <v>3</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="22">
-        <f>0.05*10^(-3) /SQRT(3)</f>
-        <v>2.8867513459481293E-5</v>
-      </c>
-      <c r="H23" s="23">
-        <v>-1.2988281250000001E-4</v>
-      </c>
-      <c r="I23" s="44">
-        <v>3.7493938379990304E-9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.6">
-      <c r="A24" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="27">
-        <v>0.05</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="25">
-        <f>0.05*10^(-3) /SQRT(3)</f>
-        <v>2.8867513459481293E-5</v>
-      </c>
-      <c r="H24" s="26">
-        <v>-1.2988281250000001E-4</v>
-      </c>
-      <c r="I24" s="45">
-        <v>3.7493938379990304E-9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="13.8">
-      <c r="A25" s="13">
-        <v>4</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="28">
-        <f>0.5 /SQRT(3)</f>
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H25" s="29">
-        <v>-2.5976562500000001E-7</v>
-      </c>
-      <c r="I25" s="44">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E26" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G26" s="31">
-        <f>0.5 /SQRT(3)</f>
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H26" s="32">
-        <v>-2.5976562500000001E-7</v>
-      </c>
-      <c r="I26" s="45">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.6">
-      <c r="A27" s="13">
-        <v>5</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="28">
-        <f>0.5 /SQRT(3)</f>
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H27" s="29">
-        <v>2.5976562500000001E-7</v>
-      </c>
-      <c r="I27" s="44">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.6">
-      <c r="A28" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="G28" s="31">
-        <f>0.5 /SQRT(3)</f>
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H28" s="32">
-        <v>2.5976562500000001E-7</v>
-      </c>
-      <c r="I28" s="45">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C29" s="35">
-        <f>1.039 *10^-5</f>
-        <v>1.039E-5</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="I29" s="46">
-        <v>3.2183031781572201E-7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="H30" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="I30" s="40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="H31" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="43">
-        <f>I29*2</f>
-        <v>6.4366063563144401E-7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="73.8">
-      <c r="A34" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="49" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="F34" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="I34" s="49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="24.6">
-      <c r="A35" s="50">
-        <v>1</v>
-      </c>
-      <c r="B35" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="50">
-        <v>125</v>
-      </c>
-      <c r="D35" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="51">
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="H35" s="52">
-        <v>8.3124999999999998E-8</v>
-      </c>
-      <c r="I35" s="52">
-        <v>4.799224112638761E-8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="24.6">
-      <c r="A36" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="C36" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="54">
-        <v>1</v>
-      </c>
-      <c r="F36" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="55">
-        <v>0.57735026918962584</v>
-      </c>
-      <c r="H36" s="56">
-        <v>8.3124999999999998E-8</v>
-      </c>
-      <c r="I36" s="57">
-        <v>4.799224112638761E-8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="24.6">
-      <c r="A37" s="50">
-        <v>2</v>
-      </c>
-      <c r="B37" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="51">
-        <v>2.8867513459481292E-9</v>
-      </c>
-      <c r="H37" s="58">
-        <v>19.53125</v>
-      </c>
-      <c r="I37" s="52">
-        <v>2.9995150703992272E-7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="24.6">
-      <c r="A38" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="53" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="59">
-        <v>0.05</v>
-      </c>
-      <c r="F38" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="55">
-        <v>2.8867513459481292E-9</v>
-      </c>
-      <c r="H38" s="60">
-        <v>19.53125</v>
-      </c>
-      <c r="I38" s="57">
-        <v>2.9995150703992272E-7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="24.6">
-      <c r="A39" s="50">
-        <v>3</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="51">
-        <v>2.8867513459481293E-5</v>
-      </c>
-      <c r="H39" s="68">
-        <v>-1.2988281250000001E-4</v>
-      </c>
-      <c r="I39" s="52">
-        <v>3.7493938379990304E-9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="24.6">
-      <c r="A40" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B40" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="61">
-        <v>0.05</v>
-      </c>
-      <c r="F40" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G40" s="55">
-        <v>2.8867513459481293E-5</v>
-      </c>
-      <c r="H40" s="69">
-        <v>-1.2988281250000001E-4</v>
-      </c>
-      <c r="I40" s="57">
-        <v>3.7493938379990304E-9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="24.6">
-      <c r="A41" s="50">
-        <v>4</v>
-      </c>
-      <c r="B41" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="50" t="s">
-        <v>130</v>
-      </c>
-      <c r="D41" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" s="51">
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H41" s="62">
-        <v>-2.5976562500000001E-7</v>
-      </c>
-      <c r="I41" s="52">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="24.6">
-      <c r="A42" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E42" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="F42" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G42" s="55">
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H42" s="64">
-        <v>-2.5976562500000001E-7</v>
-      </c>
-      <c r="I42" s="57">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="24.6">
-      <c r="A43" s="50">
-        <v>5</v>
-      </c>
-      <c r="B43" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F43" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="G43" s="51">
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H43" s="62">
-        <v>2.5976562500000001E-7</v>
-      </c>
-      <c r="I43" s="52">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="24.6">
-      <c r="A44" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="B44" s="53" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="53" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="F44" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G44" s="55">
-        <v>0.28867513459481292</v>
-      </c>
-      <c r="H44" s="64">
-        <v>2.5976562500000001E-7</v>
-      </c>
-      <c r="I44" s="57">
-        <v>7.4987876759980681E-8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="24.6">
-      <c r="A45" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="C45" s="65">
-        <v>1.039E-5</v>
-      </c>
-      <c r="D45" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="G45" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="H45" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="67">
-        <v>3.2183031781572201E-7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="H46" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="I46" s="48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="H47" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="I47" s="43">
-        <f>I45*2</f>
-        <v>6.4366063563144401E-7</v>
+    </row>
+    <row r="33" spans="8:8">
+      <c r="H33" s="48">
+        <v>6.1015800541035996E-7</v>
       </c>
     </row>
   </sheetData>
@@ -6164,6 +5918,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes on the bugdet format
</commit_message>
<xml_diff>
--- a/code/graphs.xlsx
+++ b/code/graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaled\Documents\GitHub\ThermalExpansionUncertainty\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DF716-BB00-4AC2-A0E9-3FA5CED8E873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877D9E8F-A81E-4C26-80C5-426CE1E4B7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,14 +1202,14 @@
     <numFmt numFmtId="165" formatCode="&quot;± &quot;General"/>
     <numFmt numFmtId="166" formatCode="General&quot; m&quot;"/>
     <numFmt numFmtId="167" formatCode="General&quot; m^-1 °C^-1&quot;"/>
-    <numFmt numFmtId="169" formatCode="&quot;± &quot;General&quot; mm&quot;"/>
-    <numFmt numFmtId="170" formatCode="General&quot; °C&quot;"/>
-    <numFmt numFmtId="171" formatCode="General&quot; °C^-2&quot;"/>
-    <numFmt numFmtId="172" formatCode="&quot;± &quot;General&quot; °C&quot;"/>
-    <numFmt numFmtId="173" formatCode="0.000E+00&quot; °C^-1&quot;"/>
-    <numFmt numFmtId="174" formatCode="&quot;± &quot;General\ &quot;%&quot;"/>
-    <numFmt numFmtId="178" formatCode="&quot;k= &quot;General"/>
-    <numFmt numFmtId="179" formatCode="&quot;U= &quot;General&quot; °C^-1&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;± &quot;General&quot; mm&quot;"/>
+    <numFmt numFmtId="169" formatCode="General&quot; °C&quot;"/>
+    <numFmt numFmtId="170" formatCode="General&quot; °C^-2&quot;"/>
+    <numFmt numFmtId="171" formatCode="&quot;± &quot;General&quot; °C&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.000E+00&quot; °C^-1&quot;"/>
+    <numFmt numFmtId="173" formatCode="&quot;± &quot;General\ &quot;%&quot;"/>
+    <numFmt numFmtId="174" formatCode="&quot;k= &quot;General"/>
+    <numFmt numFmtId="175" formatCode="&quot;U= &quot;General&quot; °C^-1&quot;"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -1425,7 +1425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1492,22 +1492,22 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1516,7 +1516,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1548,66 +1548,19 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3035,8 +2988,8 @@
       <xdr:rowOff>132347</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="409984" cy="347211"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -3078,6 +3031,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3125,7 +3079,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -3630,7 +3584,7 @@
         <v>1.4057954152425101E-17</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F3:F31" si="0">SQRT(E4)</f>
+        <f t="shared" ref="F4:F31" si="0">SQRT(E4)</f>
         <v>3.7493938379990304E-9</v>
       </c>
       <c r="G4" s="3"/>
@@ -5077,8 +5031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -5563,7 +5517,12 @@
         <v>6.1015800541035996E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="18" spans="1:9">
+      <c r="I18" s="50">
+        <v>47.992199999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="9" t="s">
         <v>81</v>
       </c>
@@ -5589,293 +5548,293 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" s="13">
         <v>1</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="14">
         <v>125</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="14">
         <v>0.57735026918962584</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="15">
         <v>8.3124999999999998E-8</v>
       </c>
       <c r="H20" s="43">
         <v>4.799224112638761E-8</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="52">
+      <c r="D21" s="19">
         <v>1</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="51">
+      <c r="F21" s="18">
         <v>0.57735026918962584</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="20">
         <v>8.3124999999999998E-8</v>
       </c>
       <c r="H21" s="44">
         <v>4.799224112638761E-8</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" s="13">
         <v>2</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="54">
+      <c r="F22" s="22">
         <v>2.8867513459481292E-9</v>
       </c>
-      <c r="G22" s="55">
+      <c r="G22" s="23">
         <v>19.53125</v>
       </c>
       <c r="H22" s="43">
         <v>2.8190931112774692E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="56">
+      <c r="D23" s="46">
         <v>25</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F23" s="57">
+      <c r="F23" s="24">
         <v>2.8867513459481292E-9</v>
       </c>
-      <c r="G23" s="58">
+      <c r="G23" s="25">
         <v>19.53125</v>
       </c>
       <c r="H23" s="44">
         <v>2.8190931112774692E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" s="13">
         <v>3</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B24" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F24" s="54">
+      <c r="F24" s="22">
         <v>2.8867513459481293E-5</v>
       </c>
-      <c r="G24" s="55">
+      <c r="G24" s="23">
         <v>-1.2988281250000001E-4</v>
       </c>
       <c r="H24" s="43">
         <v>3.7493938379990304E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="59">
+      <c r="D25" s="26">
         <v>0.05</v>
       </c>
-      <c r="E25" s="51" t="s">
+      <c r="E25" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="57">
+      <c r="F25" s="24">
         <v>2.8867513459481293E-5</v>
       </c>
-      <c r="G25" s="58">
+      <c r="G25" s="25">
         <v>-1.2988281250000001E-4</v>
       </c>
       <c r="H25" s="44">
         <v>3.7493938379990304E-9</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" s="13">
         <v>4</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D26" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="49" t="s">
+      <c r="E26" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="60">
+      <c r="F26" s="27">
         <v>0.28867513459481292</v>
       </c>
-      <c r="G26" s="61">
+      <c r="G26" s="28">
         <v>-2.5976562500000001E-7</v>
       </c>
       <c r="H26" s="43">
         <v>7.4987876759980681E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="29">
         <v>0.5</v>
       </c>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="63">
+      <c r="F27" s="30">
         <v>0.28867513459481292</v>
       </c>
-      <c r="G27" s="64">
+      <c r="G27" s="31">
         <v>-2.5976562500000001E-7</v>
       </c>
       <c r="H27" s="44">
         <v>7.4987876759980681E-8</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" s="13">
         <v>5</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="60">
+      <c r="F28" s="27">
         <v>0.28867513459481292</v>
       </c>
-      <c r="G28" s="61">
+      <c r="G28" s="28">
         <v>2.5976562500000001E-7</v>
       </c>
       <c r="H28" s="43">
         <v>7.4987876759980681E-8</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="29">
         <v>0.5</v>
       </c>
-      <c r="E29" s="51" t="s">
+      <c r="E29" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="63">
+      <c r="F29" s="30">
         <v>0.28867513459481292</v>
       </c>
-      <c r="G29" s="64">
+      <c r="G29" s="31">
         <v>2.5976562500000001E-7</v>
       </c>
       <c r="H29" s="44">
         <v>7.4987876759980681E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="17">
         <v>6</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="51" t="s">
+      <c r="D30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="51" t="s">
+      <c r="F30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G30" s="51" t="s">
+      <c r="G30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="H30" s="65">
+      <c r="H30" s="49">
         <v>1.9307502331381792E-8</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" s="32" t="s">
         <v>92</v>
       </c>
@@ -5901,7 +5860,7 @@
         <v>3.0507900270517998E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="H32" s="47">
         <v>2</v>
       </c>

</xml_diff>